<commit_message>
us001 task 1 closed
</commit_message>
<xml_diff>
--- a/Scrum_Backlog.xlsx
+++ b/Scrum_Backlog.xlsx
@@ -309,7 +309,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -318,28 +318,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -347,12 +329,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -367,22 +343,47 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -666,7 +667,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,63 +681,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="18" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="10" t="s">
+      <c r="D2" s="7"/>
+      <c r="E2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2" s="6">
         <v>0.5</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>15</v>
+      <c r="G2" s="31" t="s">
+        <v>34</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="14" t="s">
+      <c r="A3" s="20"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14" t="s">
+      <c r="D3" s="8"/>
+      <c r="E3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="14">
+      <c r="F3" s="8">
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -747,16 +748,16 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="14" t="s">
+      <c r="A4" s="20"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14" t="s">
+      <c r="D4" s="8"/>
+      <c r="E4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="8">
         <v>0.3</v>
       </c>
       <c r="G4" s="2" t="s">
@@ -766,15 +767,15 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="15" t="s">
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="20"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="16">
+      <c r="F5" s="10">
         <v>1</v>
       </c>
       <c r="G5" s="3" t="s">
@@ -782,16 +783,16 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="19" t="s">
+      <c r="A6" s="21"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20" t="s">
+      <c r="D6" s="12"/>
+      <c r="E6" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="21">
+      <c r="F6" s="13">
         <v>1</v>
       </c>
       <c r="G6" s="2" t="s">
@@ -799,20 +800,20 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="23" t="s">
+      <c r="D7" s="7"/>
+      <c r="E7" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="22">
+      <c r="F7" s="14">
         <v>1</v>
       </c>
       <c r="G7" s="2" t="s">
@@ -820,68 +821,68 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="24" t="s">
+      <c r="A8" s="20"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="13" t="s">
+      <c r="D8" s="8"/>
+      <c r="E8" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="23">
         <v>2</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="25" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="7"/>
+      <c r="A9" s="20"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="25"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="24" t="s">
+      <c r="A10" s="20"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="14"/>
-      <c r="E10" s="13" t="s">
+      <c r="D10" s="8"/>
+      <c r="E10" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="23">
         <v>0.3</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="25" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="7"/>
+      <c r="A11" s="20"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="25"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="14" t="s">
+      <c r="A12" s="20"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="25" t="s">
+      <c r="D12" s="8"/>
+      <c r="E12" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F12" s="14">
+      <c r="F12" s="8">
         <v>0.3</v>
       </c>
       <c r="G12" s="2" t="s">
@@ -889,16 +890,16 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="14" t="s">
+      <c r="A13" s="20"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14" t="s">
+      <c r="D13" s="8"/>
+      <c r="E13" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F13" s="14">
+      <c r="F13" s="8">
         <v>0.3</v>
       </c>
       <c r="G13" s="2" t="s">
@@ -906,16 +907,16 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="14" t="s">
+      <c r="A14" s="20"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14" t="s">
+      <c r="D14" s="8"/>
+      <c r="E14" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F14" s="14">
+      <c r="F14" s="8">
         <v>2</v>
       </c>
       <c r="G14" s="2" t="s">
@@ -923,16 +924,16 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="14" t="s">
+      <c r="A15" s="20"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14" t="s">
+      <c r="D15" s="8"/>
+      <c r="E15" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="F15" s="14">
+      <c r="F15" s="8">
         <v>1</v>
       </c>
       <c r="G15" s="2" t="s">
@@ -940,16 +941,16 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="14" t="s">
+      <c r="A16" s="20"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14" t="s">
+      <c r="D16" s="8"/>
+      <c r="E16" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F16" s="14">
+      <c r="F16" s="8">
         <v>0.5</v>
       </c>
       <c r="G16" s="2" t="s">
@@ -957,16 +958,16 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="14" t="s">
+      <c r="A17" s="20"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14" t="s">
+      <c r="D17" s="8"/>
+      <c r="E17" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F17" s="14">
+      <c r="F17" s="8">
         <v>0.5</v>
       </c>
       <c r="G17" s="2" t="s">
@@ -974,56 +975,50 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13" t="s">
+      <c r="A18" s="20"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="14"/>
-      <c r="E18" s="13" t="s">
+      <c r="D18" s="8"/>
+      <c r="E18" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="F18" s="26">
+      <c r="F18" s="24">
         <v>0.3</v>
       </c>
-      <c r="G18" s="27" t="s">
+      <c r="G18" s="26" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="28"/>
+      <c r="A19" s="20"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="27"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="17"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="20" t="s">
+      <c r="A20" s="21"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20" t="s">
+      <c r="D20" s="12"/>
+      <c r="E20" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="F20" s="20">
+      <c r="F20" s="12">
         <v>0.5</v>
       </c>
-      <c r="G20" s="29" t="s">
+      <c r="G20" s="17" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A7:A20"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="F18:F19"/>
     <mergeCell ref="G8:G9"/>
     <mergeCell ref="G10:G11"/>
     <mergeCell ref="G18:G19"/>
@@ -1034,6 +1029,12 @@
     <mergeCell ref="E10:E11"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="B7:B20"/>
+    <mergeCell ref="A7:A20"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="F18:F19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
us001 task 5 completed
</commit_message>
<xml_diff>
--- a/Scrum_Backlog.xlsx
+++ b/Scrum_Backlog.xlsx
@@ -360,42 +360,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -408,6 +372,42 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -692,7 +692,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,10 +730,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="29" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -756,8 +756,8 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="28"/>
-      <c r="B3" s="25"/>
+      <c r="A3" s="33"/>
+      <c r="B3" s="30"/>
       <c r="C3" s="7" t="s">
         <v>12</v>
       </c>
@@ -770,7 +770,7 @@
       <c r="F3" s="7">
         <v>1</v>
       </c>
-      <c r="G3" s="35" t="s">
+      <c r="G3" s="23" t="s">
         <v>33</v>
       </c>
       <c r="I3" s="3" t="s">
@@ -778,12 +778,12 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
-      <c r="B4" s="25"/>
+      <c r="A4" s="33"/>
+      <c r="B4" s="30"/>
       <c r="C4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="21" t="s">
         <v>42</v>
       </c>
       <c r="E4" s="7" t="s">
@@ -792,7 +792,7 @@
       <c r="F4" s="7">
         <v>0.3</v>
       </c>
-      <c r="G4" s="35" t="s">
+      <c r="G4" s="23" t="s">
         <v>33</v>
       </c>
       <c r="I4" s="4" t="s">
@@ -800,9 +800,9 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="34" t="s">
+      <c r="A5" s="33"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="22" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="18" t="s">
@@ -814,17 +814,17 @@
       <c r="F5" s="9">
         <v>2</v>
       </c>
-      <c r="G5" s="36" t="s">
+      <c r="G5" s="24" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="29"/>
-      <c r="B6" s="26"/>
+      <c r="A6" s="34"/>
+      <c r="B6" s="31"/>
       <c r="C6" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="37" t="s">
+      <c r="D6" s="25" t="s">
         <v>41</v>
       </c>
       <c r="E6" s="11" t="s">
@@ -833,15 +833,15 @@
       <c r="F6" s="12">
         <v>1</v>
       </c>
-      <c r="G6" s="35" t="s">
-        <v>33</v>
+      <c r="G6" s="20" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="29" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="13" t="s">
@@ -859,60 +859,60 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="28"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="30" t="s">
+      <c r="A8" s="33"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="35" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="7"/>
-      <c r="E8" s="25" t="s">
+      <c r="E8" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="31">
+      <c r="F8" s="36">
         <v>2</v>
       </c>
-      <c r="G8" s="21" t="s">
+      <c r="G8" s="26" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="28"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="30"/>
+      <c r="A9" s="33"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="35"/>
       <c r="D9" s="7"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="21"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="26"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="30" t="s">
+      <c r="A10" s="33"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="35" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="7"/>
-      <c r="E10" s="25" t="s">
+      <c r="E10" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="31">
+      <c r="F10" s="36">
         <v>0.3</v>
       </c>
-      <c r="G10" s="21" t="s">
+      <c r="G10" s="26" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="28"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="30"/>
+      <c r="A11" s="33"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="35"/>
       <c r="D11" s="7"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="21"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="26"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="28"/>
-      <c r="B12" s="25"/>
+      <c r="A12" s="33"/>
+      <c r="B12" s="30"/>
       <c r="C12" s="7" t="s">
         <v>14</v>
       </c>
@@ -928,8 +928,8 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="28"/>
-      <c r="B13" s="25"/>
+      <c r="A13" s="33"/>
+      <c r="B13" s="30"/>
       <c r="C13" s="7" t="s">
         <v>18</v>
       </c>
@@ -945,8 +945,8 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="28"/>
-      <c r="B14" s="25"/>
+      <c r="A14" s="33"/>
+      <c r="B14" s="30"/>
       <c r="C14" s="7" t="s">
         <v>22</v>
       </c>
@@ -962,8 +962,8 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="28"/>
-      <c r="B15" s="25"/>
+      <c r="A15" s="33"/>
+      <c r="B15" s="30"/>
       <c r="C15" s="7" t="s">
         <v>23</v>
       </c>
@@ -979,8 +979,8 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="28"/>
-      <c r="B16" s="25"/>
+      <c r="A16" s="33"/>
+      <c r="B16" s="30"/>
       <c r="C16" s="7" t="s">
         <v>24</v>
       </c>
@@ -996,8 +996,8 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="28"/>
-      <c r="B17" s="25"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="30"/>
       <c r="C17" s="7" t="s">
         <v>25</v>
       </c>
@@ -1013,34 +1013,34 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="28"/>
-      <c r="B18" s="25"/>
-      <c r="C18" s="25" t="s">
+      <c r="A18" s="33"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="30" t="s">
         <v>35</v>
       </c>
       <c r="D18" s="7"/>
-      <c r="E18" s="25" t="s">
+      <c r="E18" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="F18" s="32">
+      <c r="F18" s="37">
         <v>0.3</v>
       </c>
-      <c r="G18" s="22" t="s">
+      <c r="G18" s="27" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="28"/>
-      <c r="B19" s="25"/>
-      <c r="C19" s="25"/>
+      <c r="A19" s="33"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="30"/>
       <c r="D19" s="7"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="23"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="28"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="29"/>
-      <c r="B20" s="26"/>
+      <c r="A20" s="34"/>
+      <c r="B20" s="31"/>
       <c r="C20" s="11" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
US001 fully completed and Scrum_Backlog updated
</commit_message>
<xml_diff>
--- a/Scrum_Backlog.xlsx
+++ b/Scrum_Backlog.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\HospitalManagementSystem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Grp_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9617B394-9CE5-47CA-9310-C5692300E2AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -153,13 +154,13 @@
     <t>Adarsh</t>
   </si>
   <si>
-    <t>Hitesh</t>
+    <t>Harsh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -315,7 +316,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -363,10 +364,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -402,12 +408,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -688,25 +688,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="31.85546875" customWidth="1"/>
-    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" customWidth="1"/>
-    <col min="5" max="5" width="79.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.88671875" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.44140625" customWidth="1"/>
+    <col min="5" max="5" width="79.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -729,11 +729,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="29" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -755,9 +755,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="32"/>
-      <c r="B3" s="29"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="33"/>
+      <c r="B3" s="30"/>
       <c r="C3" s="7" t="s">
         <v>12</v>
       </c>
@@ -770,16 +770,16 @@
       <c r="F3" s="7">
         <v>1</v>
       </c>
-      <c r="G3" s="23" t="s">
-        <v>33</v>
+      <c r="G3" s="20" t="s">
+        <v>34</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="32"/>
-      <c r="B4" s="29"/>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="33"/>
+      <c r="B4" s="30"/>
       <c r="C4" s="7" t="s">
         <v>13</v>
       </c>
@@ -792,16 +792,16 @@
       <c r="F4" s="7">
         <v>0.3</v>
       </c>
-      <c r="G4" s="23" t="s">
-        <v>33</v>
+      <c r="G4" s="20" t="s">
+        <v>34</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="32"/>
-      <c r="B5" s="29"/>
+    <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="33"/>
+      <c r="B5" s="30"/>
       <c r="C5" s="22" t="s">
         <v>14</v>
       </c>
@@ -814,17 +814,17 @@
       <c r="F5" s="9">
         <v>2</v>
       </c>
-      <c r="G5" s="37" t="s">
+      <c r="G5" s="24" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="33"/>
-      <c r="B6" s="30"/>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="34"/>
+      <c r="B6" s="31"/>
       <c r="C6" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="23" t="s">
         <v>41</v>
       </c>
       <c r="E6" s="11" t="s">
@@ -837,11 +837,11 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="31" t="s">
+    <row r="7" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="29" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="13" t="s">
@@ -858,61 +858,61 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="32"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="34" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="33"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="38"/>
-      <c r="E8" s="29" t="s">
+      <c r="D8" s="25"/>
+      <c r="E8" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="35">
+      <c r="F8" s="36">
         <v>2</v>
       </c>
-      <c r="G8" s="25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="32"/>
-      <c r="B9" s="29"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="25"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
-      <c r="B10" s="29"/>
-      <c r="C10" s="34" t="s">
+      <c r="G8" s="26" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="33"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="26"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="33"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="38"/>
-      <c r="E10" s="29" t="s">
+      <c r="D10" s="25"/>
+      <c r="E10" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="35">
+      <c r="F10" s="36">
         <v>0.3</v>
       </c>
-      <c r="G10" s="25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="32"/>
-      <c r="B11" s="29"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="25"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
-      <c r="B12" s="29"/>
+      <c r="G10" s="26" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="33"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="26"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="33"/>
+      <c r="B12" s="30"/>
       <c r="C12" s="7" t="s">
         <v>14</v>
       </c>
@@ -927,9 +927,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
-      <c r="B13" s="29"/>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="33"/>
+      <c r="B13" s="30"/>
       <c r="C13" s="7" t="s">
         <v>18</v>
       </c>
@@ -944,9 +944,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
-      <c r="B14" s="29"/>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="33"/>
+      <c r="B14" s="30"/>
       <c r="C14" s="7" t="s">
         <v>22</v>
       </c>
@@ -961,9 +961,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="32"/>
-      <c r="B15" s="29"/>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="33"/>
+      <c r="B15" s="30"/>
       <c r="C15" s="7" t="s">
         <v>23</v>
       </c>
@@ -978,9 +978,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="32"/>
-      <c r="B16" s="29"/>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="33"/>
+      <c r="B16" s="30"/>
       <c r="C16" s="7" t="s">
         <v>24</v>
       </c>
@@ -995,9 +995,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="32"/>
-      <c r="B17" s="29"/>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="33"/>
+      <c r="B17" s="30"/>
       <c r="C17" s="7" t="s">
         <v>25</v>
       </c>
@@ -1012,35 +1012,35 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="32"/>
-      <c r="B18" s="29"/>
-      <c r="C18" s="29" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="33"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="38"/>
-      <c r="E18" s="29" t="s">
+      <c r="D18" s="25"/>
+      <c r="E18" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="F18" s="36">
+      <c r="F18" s="37">
         <v>0.3</v>
       </c>
-      <c r="G18" s="26" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="32"/>
-      <c r="B19" s="29"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="27"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="33"/>
-      <c r="B20" s="30"/>
+      <c r="G18" s="27" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="33"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="28"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="34"/>
+      <c r="B20" s="31"/>
       <c r="C20" s="11" t="s">
         <v>36</v>
       </c>
@@ -1057,12 +1057,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="G18:G19"/>
     <mergeCell ref="B2:B6"/>
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="E8:E9"/>
@@ -1073,6 +1067,12 @@
     <mergeCell ref="A7:A20"/>
     <mergeCell ref="C18:C19"/>
     <mergeCell ref="E18:E19"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="G18:G19"/>
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="F10:F11"/>
     <mergeCell ref="F18:F19"/>

</xml_diff>

<commit_message>
Final Scrum_Backlog prepared with all the tasks
</commit_message>
<xml_diff>
--- a/Scrum_Backlog.xlsx
+++ b/Scrum_Backlog.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="64">
   <si>
     <t>Story</t>
   </si>
@@ -54,9 +54,6 @@
   </si>
   <si>
     <t>Create User Login HTML Page Ref: Fig 1 Screens_HMS_Casestudy.pdf</t>
-  </si>
-  <si>
-    <t>Create HTML Page to handle Invalid Login and handle Relogin</t>
   </si>
   <si>
     <t>Task 1</t>
@@ -154,6 +151,72 @@
   </si>
   <si>
     <t>Hitesh</t>
+  </si>
+  <si>
+    <t>Task 12</t>
+  </si>
+  <si>
+    <t>Create servlet function Page to display Patient Billing Details Ref: Fig 6 Screens_HMS_Casestudy.pdf</t>
+  </si>
+  <si>
+    <t>Task 13</t>
+  </si>
+  <si>
+    <t>Create servlet function Page to Generate Patient Billing Details</t>
+  </si>
+  <si>
+    <t>US003</t>
+  </si>
+  <si>
+    <t>The functions of Pharmacists</t>
+  </si>
+  <si>
+    <t>Create DBMS Medicines Table with fields: Medicine ID, Medicine name, Quantity available, Rate of the medicine</t>
+  </si>
+  <si>
+    <t>Task 14</t>
+  </si>
+  <si>
+    <t>Task 15</t>
+  </si>
+  <si>
+    <t>Task 16</t>
+  </si>
+  <si>
+    <t>Task 17</t>
+  </si>
+  <si>
+    <t>Create DBMS Patient_Medicines Table with fields:Patient ID, ID of Medicine issued, Quantity issued</t>
+  </si>
+  <si>
+    <t>Create DBMS Patient_Diagnostics Table with fields: Patient ID, ID of Test conducted</t>
+  </si>
+  <si>
+    <t>Create HTML Page to handle Invalid Login and handle Re login</t>
+  </si>
+  <si>
+    <t>Create HTML Page to Search Patient Ref: 5.3.1 in SRS. Display error message on failure.</t>
+  </si>
+  <si>
+    <t>Create HTML Issue Medicines Screen Ref: 5.2.2. in SRS. Display error message on failure.</t>
+  </si>
+  <si>
+    <t>Create servlet function Page to issue medicines</t>
+  </si>
+  <si>
+    <t>US004</t>
+  </si>
+  <si>
+    <t>The functions of Diagnostics</t>
+  </si>
+  <si>
+    <t>Create HTML Page to Search Patient Ref: 5.2.1 in SRS. Display error message on failure.</t>
+  </si>
+  <si>
+    <t>Create HTML Diagnostics Screen Ref: 5.3.2. in SRS. Display error message on failure.</t>
+  </si>
+  <si>
+    <t>Create servlet function Page to issue diagnostic tests</t>
   </si>
 </sst>
 </file>
@@ -315,10 +378,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -327,9 +389,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -350,16 +409,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -367,11 +417,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -397,17 +459,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -689,10 +759,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -707,375 +777,622 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="15" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="31"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D3" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="6">
+        <v>1</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="31"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="31"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="7">
+        <v>2</v>
+      </c>
+      <c r="G5" s="23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="32"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="10">
+        <v>1</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="24"/>
+      <c r="E7" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F7" s="22">
         <v>0.5</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G7" s="36" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="31"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="24"/>
+      <c r="E8" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="G8" s="37" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="31"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="24"/>
+      <c r="F9" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="G9" s="37" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="31"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="24"/>
+      <c r="E10" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="G10" s="37" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="31"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="G11" s="37" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="31"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="25"/>
+      <c r="E12" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="34">
+        <v>2</v>
+      </c>
+      <c r="G12" s="26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="31"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="26"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="31"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="25"/>
+      <c r="E14" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="34">
+        <v>0.3</v>
+      </c>
+      <c r="G14" s="26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="31"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="26"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="31"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="G16" s="36" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="31"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="G17" s="36" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="31"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="32"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="7" t="s">
+      <c r="D18" s="6"/>
+      <c r="E18" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" s="6">
+        <v>2</v>
+      </c>
+      <c r="G18" s="36" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="31"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" s="6">
+        <v>1</v>
+      </c>
+      <c r="G19" s="36" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="31"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="G20" s="36" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="31"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="G21" s="36" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="31"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="25"/>
+      <c r="E22" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="F22" s="34">
+        <v>0.3</v>
+      </c>
+      <c r="G22" s="26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="31"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="34"/>
+      <c r="G23" s="26"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="31"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F24" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="G24" s="36" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="31"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" s="6"/>
+      <c r="E25" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="F25" s="35">
+        <v>0.3</v>
+      </c>
+      <c r="G25" s="36" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="32"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F26" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="G26" s="14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="4"/>
+      <c r="E27" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="F27" s="41">
+        <v>1</v>
+      </c>
+      <c r="G27" s="37" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="42"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" s="6"/>
+      <c r="E28" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F28" s="35">
+        <v>1</v>
+      </c>
+      <c r="G28" s="36" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="42"/>
+      <c r="B29" s="28"/>
+      <c r="C29" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="7">
+      <c r="D29" s="6"/>
+      <c r="E29" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F29" s="35">
         <v>1</v>
       </c>
-      <c r="G3" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="32"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="7" t="s">
+      <c r="G29" s="36" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="43"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4" s="7" t="s">
+      <c r="D30" s="9"/>
+      <c r="E30" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F30" s="38">
+        <v>1</v>
+      </c>
+      <c r="G30" s="14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="7">
-        <v>0.3</v>
-      </c>
-      <c r="G4" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="32"/>
-      <c r="B5" s="29"/>
-      <c r="C5" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="9">
-        <v>2</v>
-      </c>
-      <c r="G5" s="37" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="33"/>
-      <c r="B6" s="30"/>
-      <c r="C6" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="12">
+      <c r="D31" s="4"/>
+      <c r="E31" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F31" s="41">
         <v>1</v>
       </c>
-      <c r="G6" s="20" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="13" t="s">
+      <c r="G31" s="37" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="42"/>
+      <c r="B32" s="28"/>
+      <c r="C32" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" s="13">
+      <c r="D32" s="6"/>
+      <c r="E32" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F32" s="35">
         <v>1</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="32"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="34" t="s">
+      <c r="G32" s="36" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="42"/>
+      <c r="B33" s="28"/>
+      <c r="C33" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="38"/>
-      <c r="E8" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="35">
-        <v>2</v>
-      </c>
-      <c r="G8" s="25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="32"/>
-      <c r="B9" s="29"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="25"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
-      <c r="B10" s="29"/>
-      <c r="C10" s="34" t="s">
+      <c r="D33" s="6"/>
+      <c r="E33" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F33" s="35">
+        <v>1</v>
+      </c>
+      <c r="G33" s="36" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="43"/>
+      <c r="B34" s="29"/>
+      <c r="C34" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="38"/>
-      <c r="E10" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" s="35">
-        <v>0.3</v>
-      </c>
-      <c r="G10" s="25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="32"/>
-      <c r="B11" s="29"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="25"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
-      <c r="B12" s="29"/>
-      <c r="C12" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" s="7">
-        <v>0.3</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
-      <c r="B13" s="29"/>
-      <c r="C13" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F13" s="7">
-        <v>0.3</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
-      <c r="B14" s="29"/>
-      <c r="C14" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F14" s="7">
-        <v>2</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="32"/>
-      <c r="B15" s="29"/>
-      <c r="C15" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" s="7">
+      <c r="D34" s="9"/>
+      <c r="E34" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F34" s="38">
         <v>1</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="32"/>
-      <c r="B16" s="29"/>
-      <c r="C16" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="F16" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="32"/>
-      <c r="B17" s="29"/>
-      <c r="C17" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F17" s="7">
-        <v>0.5</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="32"/>
-      <c r="B18" s="29"/>
-      <c r="C18" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" s="38"/>
-      <c r="E18" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="F18" s="36">
-        <v>0.3</v>
-      </c>
-      <c r="G18" s="26" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="32"/>
-      <c r="B19" s="29"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="27"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="33"/>
-      <c r="B20" s="30"/>
-      <c r="C20" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="F20" s="11">
-        <v>0.5</v>
-      </c>
-      <c r="G20" s="16" t="s">
-        <v>15</v>
+      <c r="G34" s="14" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="G18:G19"/>
+  <mergeCells count="23">
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="B31:B34"/>
     <mergeCell ref="B2:B6"/>
     <mergeCell ref="A2:A6"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="B7:B20"/>
-    <mergeCell ref="A7:A20"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="A7:A26"/>
+    <mergeCell ref="B7:B26"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="F22:F23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
us002 task 1,2,3,4,5 completed.
</commit_message>
<xml_diff>
--- a/Scrum_Backlog.xlsx
+++ b/Scrum_Backlog.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="65">
   <si>
     <t>Story</t>
   </si>
@@ -216,10 +216,10 @@
     <t>Harsh</t>
   </si>
   <si>
-    <t>Create DBMS Diagonstic Table with fields: Medicine ID, Medicine name, Quantity available, Rate of the medicine</t>
-  </si>
-  <si>
     <t>Create HTML Page to display Patient Billing Details Ref: Fig 6 Screens_HMS_Casestudy.pdf</t>
+  </si>
+  <si>
+    <t>Create DBMS Diagonstic Table with fields: test id, name of test, price of test</t>
   </si>
 </sst>
 </file>
@@ -381,7 +381,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -451,12 +451,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -478,18 +496,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -772,8 +780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -811,10 +819,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="40" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -837,8 +845,8 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="40"/>
-      <c r="B3" s="34"/>
+      <c r="A3" s="46"/>
+      <c r="B3" s="37"/>
       <c r="C3" s="6" t="s">
         <v>11</v>
       </c>
@@ -859,8 +867,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="40"/>
-      <c r="B4" s="34"/>
+      <c r="A4" s="46"/>
+      <c r="B4" s="37"/>
       <c r="C4" s="6" t="s">
         <v>12</v>
       </c>
@@ -881,8 +889,8 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="40"/>
-      <c r="B5" s="34"/>
+      <c r="A5" s="46"/>
+      <c r="B5" s="37"/>
       <c r="C5" s="17" t="s">
         <v>13</v>
       </c>
@@ -900,8 +908,8 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="41"/>
-      <c r="B6" s="35"/>
+      <c r="A6" s="47"/>
+      <c r="B6" s="41"/>
       <c r="C6" s="8" t="s">
         <v>17</v>
       </c>
@@ -919,157 +927,167 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="40" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="23"/>
+      <c r="D7" s="23" t="s">
+        <v>40</v>
+      </c>
       <c r="E7" s="12" t="s">
         <v>39</v>
       </c>
       <c r="F7" s="21">
         <v>0.5</v>
       </c>
-      <c r="G7" s="25" t="s">
-        <v>14</v>
+      <c r="G7" s="48" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="40"/>
-      <c r="B8" s="34"/>
+      <c r="A8" s="46"/>
+      <c r="B8" s="37"/>
       <c r="C8" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="23"/>
+      <c r="D8" s="23" t="s">
+        <v>40</v>
+      </c>
       <c r="E8" s="28" t="s">
         <v>46</v>
       </c>
       <c r="F8" s="21">
         <v>0.5</v>
       </c>
-      <c r="G8" s="26" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="40"/>
-      <c r="B9" s="34"/>
+      <c r="G8" s="49" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="46"/>
+      <c r="B9" s="37"/>
       <c r="C9" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="23"/>
+      <c r="D9" s="23" t="s">
+        <v>40</v>
+      </c>
       <c r="E9" s="28" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F9" s="7">
         <v>0.5</v>
       </c>
-      <c r="G9" s="26" t="s">
-        <v>14</v>
+      <c r="G9" s="49" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="40"/>
-      <c r="B10" s="34"/>
+      <c r="A10" s="46"/>
+      <c r="B10" s="37"/>
       <c r="C10" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="31"/>
+      <c r="D10" s="31" t="s">
+        <v>40</v>
+      </c>
       <c r="E10" s="28" t="s">
         <v>51</v>
       </c>
       <c r="F10" s="7">
         <v>0.5</v>
       </c>
-      <c r="G10" s="26" t="s">
-        <v>14</v>
+      <c r="G10" s="49" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="40"/>
-      <c r="B11" s="34"/>
+      <c r="A11" s="46"/>
+      <c r="B11" s="37"/>
       <c r="C11" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="30"/>
+      <c r="D11" s="30" t="s">
+        <v>40</v>
+      </c>
       <c r="E11" s="28" t="s">
         <v>52</v>
       </c>
       <c r="F11" s="7">
         <v>0.5</v>
       </c>
-      <c r="G11" s="26" t="s">
-        <v>14</v>
+      <c r="G11" s="49" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="40"/>
-      <c r="B12" s="34"/>
-      <c r="C12" s="42" t="s">
+      <c r="A12" s="46"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="43" t="s">
+      <c r="D12" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="E12" s="34" t="s">
+      <c r="E12" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="45">
+      <c r="F12" s="36">
         <v>2</v>
       </c>
-      <c r="G12" s="44" t="s">
+      <c r="G12" s="35" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="40"/>
-      <c r="B13" s="34"/>
-      <c r="C13" s="42"/>
-      <c r="D13" s="43"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="45"/>
-      <c r="G13" s="44"/>
+      <c r="A13" s="46"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="35"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="40"/>
-      <c r="B14" s="34"/>
-      <c r="C14" s="42" t="s">
+      <c r="A14" s="46"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="43" t="s">
+      <c r="D14" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="E14" s="34" t="s">
+      <c r="E14" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="45">
+      <c r="F14" s="36">
         <v>0.3</v>
       </c>
-      <c r="G14" s="44" t="s">
+      <c r="G14" s="35" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="40"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="42"/>
-      <c r="D15" s="43"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="45"/>
-      <c r="G15" s="44"/>
+      <c r="A15" s="46"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="35"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="40"/>
-      <c r="B16" s="34"/>
+      <c r="A16" s="46"/>
+      <c r="B16" s="37"/>
       <c r="C16" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="33" t="s">
         <v>62</v>
       </c>
       <c r="E16" s="13" t="s">
@@ -1083,12 +1101,12 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="40"/>
-      <c r="B17" s="34"/>
+      <c r="A17" s="46"/>
+      <c r="B17" s="37"/>
       <c r="C17" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="34" t="s">
         <v>62</v>
       </c>
       <c r="E17" s="6" t="s">
@@ -1102,8 +1120,8 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="40"/>
-      <c r="B18" s="34"/>
+      <c r="A18" s="46"/>
+      <c r="B18" s="37"/>
       <c r="C18" s="6" t="s">
         <v>34</v>
       </c>
@@ -1119,8 +1137,8 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="40"/>
-      <c r="B19" s="34"/>
+      <c r="A19" s="46"/>
+      <c r="B19" s="37"/>
       <c r="C19" s="6" t="s">
         <v>35</v>
       </c>
@@ -1136,8 +1154,8 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="40"/>
-      <c r="B20" s="34"/>
+      <c r="A20" s="46"/>
+      <c r="B20" s="37"/>
       <c r="C20" s="6" t="s">
         <v>41</v>
       </c>
@@ -1153,8 +1171,8 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="40"/>
-      <c r="B21" s="34"/>
+      <c r="A21" s="46"/>
+      <c r="B21" s="37"/>
       <c r="C21" s="6" t="s">
         <v>42</v>
       </c>
@@ -1170,36 +1188,36 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="40"/>
-      <c r="B22" s="34"/>
-      <c r="C22" s="34" t="s">
+      <c r="A22" s="46"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="43" t="s">
+      <c r="D22" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="E22" s="34" t="s">
+      <c r="E22" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="F22" s="45">
+      <c r="F22" s="36">
         <v>0.3</v>
       </c>
-      <c r="G22" s="44" t="s">
+      <c r="G22" s="35" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="40"/>
-      <c r="B23" s="34"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="43"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="45"/>
-      <c r="G23" s="44"/>
+      <c r="A23" s="46"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="35"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="40"/>
-      <c r="B24" s="34"/>
+      <c r="A24" s="46"/>
+      <c r="B24" s="37"/>
       <c r="C24" s="6" t="s">
         <v>48</v>
       </c>
@@ -1215,8 +1233,8 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="40"/>
-      <c r="B25" s="34"/>
+      <c r="A25" s="46"/>
+      <c r="B25" s="37"/>
       <c r="C25" s="24" t="s">
         <v>49</v>
       </c>
@@ -1224,7 +1242,7 @@
         <v>62</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F25" s="24">
         <v>0.3</v>
@@ -1234,8 +1252,8 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="41"/>
-      <c r="B26" s="35"/>
+      <c r="A26" s="47"/>
+      <c r="B26" s="41"/>
       <c r="C26" s="27" t="s">
         <v>50</v>
       </c>
@@ -1251,10 +1269,10 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="B27" s="33" t="s">
+      <c r="B27" s="40" t="s">
         <v>45</v>
       </c>
       <c r="C27" s="29" t="s">
@@ -1272,8 +1290,8 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="37"/>
-      <c r="B28" s="34"/>
+      <c r="A28" s="43"/>
+      <c r="B28" s="37"/>
       <c r="C28" s="24" t="s">
         <v>11</v>
       </c>
@@ -1289,8 +1307,8 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="37"/>
-      <c r="B29" s="34"/>
+      <c r="A29" s="43"/>
+      <c r="B29" s="37"/>
       <c r="C29" s="24" t="s">
         <v>12</v>
       </c>
@@ -1306,8 +1324,8 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="38"/>
-      <c r="B30" s="35"/>
+      <c r="A30" s="44"/>
+      <c r="B30" s="41"/>
       <c r="C30" s="27" t="s">
         <v>13</v>
       </c>
@@ -1323,10 +1341,10 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="36" t="s">
+      <c r="A31" s="42" t="s">
         <v>57</v>
       </c>
-      <c r="B31" s="33" t="s">
+      <c r="B31" s="40" t="s">
         <v>58</v>
       </c>
       <c r="C31" s="29" t="s">
@@ -1344,8 +1362,8 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="37"/>
-      <c r="B32" s="34"/>
+      <c r="A32" s="43"/>
+      <c r="B32" s="37"/>
       <c r="C32" s="24" t="s">
         <v>11</v>
       </c>
@@ -1361,8 +1379,8 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="37"/>
-      <c r="B33" s="34"/>
+      <c r="A33" s="43"/>
+      <c r="B33" s="37"/>
       <c r="C33" s="24" t="s">
         <v>12</v>
       </c>
@@ -1378,8 +1396,8 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="38"/>
-      <c r="B34" s="35"/>
+      <c r="A34" s="44"/>
+      <c r="B34" s="41"/>
       <c r="C34" s="27" t="s">
         <v>13</v>
       </c>
@@ -1396,12 +1414,14 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:A26"/>
+    <mergeCell ref="B7:B26"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="E14:E15"/>
@@ -1411,14 +1431,12 @@
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="D22:D23"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="B2:B6"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A7:A26"/>
-    <mergeCell ref="B7:B26"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="F22:F23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>